<commit_message>
Corrections in hardware - now rev. E
</commit_message>
<xml_diff>
--- a/Hardware/calculation.xlsx
+++ b/Hardware/calculation.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a13dfe35cafc0b17/Thiago/Projetos/Z80 Computer/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a13dfe35cafc0b17/Thiago/Projetos/Z80 Computer/Hardware/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="83" documentId="8_{D4285107-DC1E-4674-BF63-9FD7B0170529}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B2F63CF9-4AA8-4E39-8DD7-729BDD3BDE8D}"/>
+  <xr:revisionPtr revIDLastSave="106" documentId="8_{D4285107-DC1E-4674-BF63-9FD7B0170529}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3162C0ED-3147-49DF-920D-FB12B39347E7}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F322F79A-C795-48CC-841F-20B5E223CB2E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{F322F79A-C795-48CC-841F-20B5E223CB2E}"/>
   </bookViews>
   <sheets>
-    <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
+    <sheet name="Clock_555" sheetId="1" r:id="rId1"/>
+    <sheet name="Clock_NOT_logic" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>hFE</t>
   </si>
@@ -75,6 +76,12 @@
   </si>
   <si>
     <t>Timer 555 - Gerador de Clock</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>R</t>
   </si>
 </sst>
 </file>
@@ -308,6 +315,116 @@
         <a:xfrm>
           <a:off x="13653692" y="2647949"/>
           <a:ext cx="2396445" cy="3896557"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>153251</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagem 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D83AB1AB-D1DE-EB69-763C-7EB165E28E30}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="4972050" y="781050"/>
+          <a:ext cx="3362325" cy="1848701"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>35780</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagem 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9B1FD37F-5B67-6D83-422C-851FD47592D5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5172075" y="2714625"/>
+          <a:ext cx="2828925" cy="1702655"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -618,7 +735,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A61E7BEE-D955-48DA-8D0B-1AFC975AA769}">
   <dimension ref="E4:K20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
@@ -750,4 +867,45 @@
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8A24528-F4FC-434C-A128-D57E38BBB453}">
+  <dimension ref="C7:D9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="7" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="2">
+        <f>1/(2.2*D8*D9)</f>
+        <v>454.5454545454545</v>
+      </c>
+    </row>
+    <row r="8" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="1">
+        <v>9.9999999999999995E-7</v>
+      </c>
+    </row>
+    <row r="9" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="1">
+        <v>1000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>